<commit_message>
resistant Tuberculosis health burden
</commit_message>
<xml_diff>
--- a/data/Vaccine profile age_assumptions - CL edit.xlsx
+++ b/data/Vaccine profile age_assumptions - CL edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ivionline-my.sharepoint.com/personal/chaelin_kim_ivi_int/Documents/Documents/GitHub/vaccine_amr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{BB449E5E-4C08-C340-B34F-4BD61F62AC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BFD8BD2-BA3B-417A-A745-B0CAC57F61EF}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{BB449E5E-4C08-C340-B34F-4BD61F62AC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36F82098-08C0-4180-85B2-7BEA8E350E0F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6525" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3505429-E9FF-3944-B32E-F1BA65C67D7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E3505429-E9FF-3944-B32E-F1BA65C67D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="SIGs" sheetId="1" state="hidden" r:id="rId1"/>
@@ -30,6 +30,65 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Chaelin Kim</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{87A771A0-DC78-4CC7-A676-CABE6E075772}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Chaelin Kim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+starting
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{26B1D8AB-1655-4466-A662-3425562BE23F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Chaelin Kim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+less than</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="363">
   <si>
@@ -2444,12 +2503,6 @@
     <t>Clostridioides difficile</t>
   </si>
   <si>
-    <t>Start_age</t>
-  </si>
-  <si>
-    <t>End_age</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -2476,13 +2529,19 @@
   <si>
     <t>•Immunocompromised patients and/or suffering from co-morbidities
 •hospital patients undergoing elective surgery or other invasive procedures with high risk of S. aureus infection</t>
+  </si>
+  <si>
+    <t>Start_age</t>
+  </si>
+  <si>
+    <t>End_age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2563,6 +2622,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4739,12 +4811,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9E86CB-7D0A-7349-B091-299D92D6946C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9E86CB-7D0A-7349-B091-299D92D6946C}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4782,13 +4854,13 @@
         <v>247</v>
       </c>
       <c r="I1" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="K1" s="48" t="s">
         <v>352</v>
-      </c>
-      <c r="J1" s="47" t="s">
-        <v>353</v>
-      </c>
-      <c r="K1" s="48" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="156" x14ac:dyDescent="0.3">
@@ -4820,10 +4892,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="156" x14ac:dyDescent="0.3">
@@ -4855,10 +4927,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K3" s="51" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="109.2" x14ac:dyDescent="0.3">
@@ -5004,10 +5076,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K8" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="109.2" x14ac:dyDescent="0.3">
@@ -5039,10 +5111,10 @@
         <v>0.5</v>
       </c>
       <c r="J9" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="52" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5065,7 +5137,7 @@
         <v>257</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H10" s="42" t="s">
         <v>236</v>
@@ -5074,10 +5146,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5100,7 +5172,7 @@
         <v>257</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H11" s="42" t="s">
         <v>236</v>
@@ -5109,10 +5181,10 @@
         <v>60</v>
       </c>
       <c r="J11" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K11" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5144,10 +5216,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K12" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="78" x14ac:dyDescent="0.3">
@@ -5179,10 +5251,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5214,10 +5286,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
@@ -5365,10 +5437,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="57">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K19" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="171.6" x14ac:dyDescent="0.3">
@@ -5400,10 +5472,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K20" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="78" x14ac:dyDescent="0.3">
@@ -5522,10 +5594,10 @@
         <v>10</v>
       </c>
       <c r="J24" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K24" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
@@ -5557,10 +5629,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K25" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="93.6" x14ac:dyDescent="0.3">
@@ -5650,10 +5722,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K28" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
@@ -5714,10 +5786,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K30" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="78" x14ac:dyDescent="0.3">
@@ -5926,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5949,7 +6021,7 @@
         <v>300</v>
       </c>
       <c r="G38" s="42" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H38" s="42" t="s">
         <v>236</v>
@@ -5958,10 +6030,10 @@
         <v>0.5</v>
       </c>
       <c r="J38" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K38" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
@@ -5984,7 +6056,7 @@
         <v>300</v>
       </c>
       <c r="G39" s="42" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H39" s="42" t="s">
         <v>236</v>
@@ -5993,10 +6065,10 @@
         <v>60</v>
       </c>
       <c r="J39" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K39" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="156" x14ac:dyDescent="0.3">
@@ -6019,7 +6091,7 @@
         <v>300</v>
       </c>
       <c r="G40" s="42" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H40" s="42" t="s">
         <v>236</v>
@@ -6028,10 +6100,10 @@
         <v>0</v>
       </c>
       <c r="J40" s="50">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K40" s="51" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="109.2" x14ac:dyDescent="0.3">
@@ -6063,10 +6135,10 @@
         <v>0</v>
       </c>
       <c r="J41" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="109.2" x14ac:dyDescent="0.3">
@@ -6098,10 +6170,10 @@
         <v>0</v>
       </c>
       <c r="J42" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K42" s="51" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
@@ -6140,6 +6212,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>